<commit_message>
Added raise of clean_df function
</commit_message>
<xml_diff>
--- a/data/dicts/other_codes.xlsx
+++ b/data/dicts/other_codes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>Отказано в авторизации</t>
   </si>
@@ -76,6 +76,33 @@
   </si>
   <si>
     <t>Внутренняя ошибка сервера</t>
+  </si>
+  <si>
+    <t>Неудовлетворительное качество БО</t>
+  </si>
+  <si>
+    <t>Ошибка при взаимодействии с ФХ СМЭВ</t>
+  </si>
+  <si>
+    <t>Ошибка валидации логина пароля ФХ СМЭВ</t>
+  </si>
+  <si>
+    <t>Проблемы взаимодействия со СМЭВ (агрегированная ошибка)</t>
+  </si>
+  <si>
+    <t>ИСКО</t>
+  </si>
+  <si>
+    <t>ЕБС</t>
+  </si>
+  <si>
+    <t>ЕСИА</t>
+  </si>
+  <si>
+    <t>СМЭВ</t>
+  </si>
+  <si>
+    <t>ИГНОРИРОВАТЬ</t>
   </si>
 </sst>
 </file>
@@ -393,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,156 +431,254 @@
     <col min="1" max="1" width="48.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
         <v>401</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>402</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>404</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <v>406</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
         <v>408</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
         <v>409</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7">
         <v>410</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8">
         <v>411</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9">
         <v>412</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10">
         <v>413</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11">
         <v>414</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12">
         <v>415</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13">
         <v>416</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14">
         <v>417</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15">
         <v>418</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16">
         <v>419</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17">
         <v>420</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18">
         <v>421</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>422</v>
+      </c>
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>432</v>
+      </c>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>433</v>
+      </c>
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>18</v>
       </c>
-      <c r="B19">
+      <c r="B22">
         <v>500</v>
+      </c>
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>505</v>
       </c>
     </row>
   </sheetData>

</xml_diff>